<commit_message>
Added handling of calendar for school year, and attendance tables.
</commit_message>
<xml_diff>
--- a/TESTDATA/RESOURCES/templates/Vorlage_Klassenbuch.xlsx
+++ b/TESTDATA/RESOURCES/templates/Vorlage_Klassenbuch.xlsx
@@ -15,48 +15,6 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Info!$B:$C</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Info!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Monat!$B:$C</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -68,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -104,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">*f1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasse:</t>
   </si>
   <si>
     <t xml:space="preserve">{Klasse}</t>
@@ -257,9 +218,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -280,87 +241,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -418,13 +298,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="0"/>
@@ -465,54 +338,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -528,32 +359,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -613,7 +435,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -637,56 +459,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -695,23 +469,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,193 +501,173 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -941,7 +695,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -964,26 +718,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ65536"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="11" style="0" width="3.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="34" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1451,7 +1204,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1477,33 +1230,35 @@
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="N3" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="O3" s="16"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18" t="s">
+      <c r="P3" s="16"/>
+      <c r="Q3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="19" t="s">
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17" t="s">
         <v>15</v>
       </c>
+      <c r="V3" s="17"/>
+      <c r="W3" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="X3" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Y3" s="16"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-    </row>
-    <row r="4" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+    </row>
+    <row r="4" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1512,10 +1267,10 @@
       <c r="I4" s="5"/>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1523,26 +1278,26 @@
       <c r="H5" s="15"/>
       <c r="I5" s="5"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="24" t="s">
+      <c r="K5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-    </row>
-    <row r="6" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+    </row>
+    <row r="6" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1550,26 +1305,26 @@
       <c r="H6" s="15"/>
       <c r="I6" s="5"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="24" t="s">
+      <c r="K6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-    </row>
-    <row r="7" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M6" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+    </row>
+    <row r="7" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1577,26 +1332,26 @@
       <c r="H7" s="15"/>
       <c r="I7" s="5"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="24" t="s">
+      <c r="K7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-    </row>
-    <row r="8" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M7" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+    </row>
+    <row r="8" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1604,26 +1359,26 @@
       <c r="H8" s="15"/>
       <c r="I8" s="5"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="24" t="s">
+      <c r="K8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-    </row>
-    <row r="9" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+    </row>
+    <row r="9" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1632,10 +1387,10 @@
       <c r="I9" s="5"/>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="15"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1643,14 +1398,14 @@
       <c r="H10" s="15"/>
       <c r="I10" s="5"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="28"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
+      <c r="K10" s="27"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
@@ -1658,10 +1413,10 @@
       <c r="AB10" s="15"/>
       <c r="AC10" s="15"/>
     </row>
-    <row r="11" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="15"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -1669,15 +1424,15 @@
       <c r="H11" s="15"/>
       <c r="I11" s="5"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
+      <c r="K11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
@@ -1691,10 +1446,10 @@
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
     </row>
-    <row r="12" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1722,10 +1477,10 @@
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
     </row>
-    <row r="13" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="15"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1733,23 +1488,23 @@
       <c r="H13" s="15"/>
       <c r="I13" s="5"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
@@ -1757,10 +1512,10 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
     </row>
-    <row r="14" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1768,23 +1523,23 @@
       <c r="H14" s="15"/>
       <c r="I14" s="5"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="30"/>
-      <c r="M14" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
@@ -1792,10 +1547,10 @@
       <c r="AB14" s="15"/>
       <c r="AC14" s="15"/>
     </row>
-    <row r="15" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1803,34 +1558,34 @@
       <c r="H15" s="15"/>
       <c r="I15" s="5"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="30"/>
-      <c r="M15" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-    </row>
-    <row r="16" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L15" s="29"/>
+      <c r="M15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
+    </row>
+    <row r="16" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1838,23 +1593,23 @@
       <c r="H16" s="15"/>
       <c r="I16" s="5"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="30" t="s">
+      <c r="K16" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="L16" s="30"/>
-      <c r="M16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
       <c r="X16" s="15"/>
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
@@ -1862,10 +1617,10 @@
       <c r="AB16" s="15"/>
       <c r="AC16" s="15"/>
     </row>
-    <row r="17" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="15"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1873,23 +1628,23 @@
       <c r="H17" s="15"/>
       <c r="I17" s="5"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="30" t="n">
+      <c r="K17" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
@@ -1897,10 +1652,10 @@
       <c r="AB17" s="15"/>
       <c r="AC17" s="15"/>
     </row>
-    <row r="18" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1908,23 +1663,23 @@
       <c r="H18" s="15"/>
       <c r="I18" s="5"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="30"/>
-      <c r="M18" s="24" t="s">
+      <c r="K18" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
@@ -1932,10 +1687,10 @@
       <c r="AB18" s="15"/>
       <c r="AC18" s="15"/>
     </row>
-    <row r="19" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1963,10 +1718,10 @@
       <c r="AB19" s="15"/>
       <c r="AC19" s="15"/>
     </row>
-    <row r="20" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1993,13 +1748,13 @@
       <c r="AA20" s="15"/>
       <c r="AB20" s="15"/>
       <c r="AC20" s="15"/>
-      <c r="AF20" s="24"/>
-      <c r="AG20" s="24"/>
-    </row>
-    <row r="21" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="23"/>
+    </row>
+    <row r="21" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -2007,18 +1762,18 @@
       <c r="H21" s="15"/>
       <c r="I21" s="5"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
+      <c r="K21" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
       <c r="U21" s="15"/>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
@@ -2028,13 +1783,13 @@
       <c r="AA21" s="15"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="15"/>
-      <c r="AF21" s="24"/>
-      <c r="AG21" s="24"/>
-    </row>
-    <row r="22" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+    </row>
+    <row r="22" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="15"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -2042,36 +1797,36 @@
       <c r="H22" s="15"/>
       <c r="I22" s="5"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="30"/>
-      <c r="M22" s="24" t="s">
+      <c r="K22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-    </row>
-    <row r="23" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L22" s="29"/>
+      <c r="M22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+    </row>
+    <row r="23" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="15"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -2079,36 +1834,36 @@
       <c r="H23" s="15"/>
       <c r="I23" s="5"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="L23" s="30"/>
-      <c r="M23" s="24" t="s">
+      <c r="K23" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-    </row>
-    <row r="24" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L23" s="29"/>
+      <c r="M23" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+    </row>
+    <row r="24" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="15"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -2116,34 +1871,34 @@
       <c r="H24" s="15"/>
       <c r="I24" s="5"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="L24" s="30"/>
-      <c r="M24" s="24" t="s">
+      <c r="K24" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
       <c r="AA24" s="15"/>
       <c r="AB24" s="15"/>
       <c r="AC24" s="15"/>
     </row>
-    <row r="25" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="15"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -2151,34 +1906,34 @@
       <c r="H25" s="15"/>
       <c r="I25" s="5"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" s="30"/>
-      <c r="M25" s="24" t="s">
+      <c r="K25" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
       <c r="AA25" s="15"/>
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
     </row>
-    <row r="26" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="15"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -2186,23 +1941,23 @@
       <c r="H26" s="15"/>
       <c r="I26" s="5"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="30"/>
-      <c r="M26" s="24" t="s">
+      <c r="K26" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
       <c r="X26" s="15"/>
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
@@ -2210,10 +1965,10 @@
       <c r="AB26" s="15"/>
       <c r="AC26" s="15"/>
     </row>
-    <row r="27" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="15"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -2241,10 +1996,10 @@
       <c r="AB27" s="15"/>
       <c r="AC27" s="15"/>
     </row>
-    <row r="28" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="15"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -2252,21 +2007,21 @@
       <c r="H28" s="15"/>
       <c r="I28" s="5"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
+      <c r="K28" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
@@ -2274,65 +2029,65 @@
       <c r="AB28" s="15"/>
       <c r="AC28" s="15"/>
     </row>
-    <row r="29" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="32"/>
+    <row r="29" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="31"/>
       <c r="I29" s="5"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
-      <c r="U29" s="31"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="31"/>
-    </row>
-    <row r="30" s="20" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="32"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+    </row>
+    <row r="30" s="19" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="31"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="32"/>
+    <row r="31" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="31"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="32"/>
+    <row r="32" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="31"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32"/>
+    <row r="33" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="31"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32"/>
+    <row r="34" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="31"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32"/>
+    <row r="35" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="32"/>
+    <row r="36" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="31"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="32"/>
+    <row r="37" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="31"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="32"/>
+    <row r="38" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="31"/>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="32"/>
+    <row r="39" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="32"/>
+    <row r="40" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31"/>
       <c r="I40" s="5"/>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2353,10 +2108,11 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="X3:Y3"/>
@@ -2390,38 +2146,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ4"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="4" style="0" width="3.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="37" style="0" width="4.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="42" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>34</v>
+      <c r="C1" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="E1" s="13" t="n">
         <v>1</v>
@@ -2516,8 +2271,8 @@
       <c r="AI1" s="13" t="n">
         <v>31</v>
       </c>
-      <c r="AJ1" s="36" t="s">
-        <v>48</v>
+      <c r="AJ1" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="AK1" s="4" t="s">
         <v>1</v>
@@ -2919,8 +2674,8 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>49</v>
+      <c r="A2" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>7</v>
@@ -2928,60 +2683,60 @@
       <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="38"/>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
       <c r="AN2" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AO2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="C3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="40"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -3013,7 +2768,7 @@
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
       <c r="AI3" s="4"/>
-      <c r="AJ3" s="41"/>
+      <c r="AJ3" s="40"/>
       <c r="AK3" s="4" t="s">
         <v>11</v>
       </c>
@@ -3027,7 +2782,7 @@
         <v>11</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3049,7 +2804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3059,361 +2814,360 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="44"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="44"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="44"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>